<commit_message>
Start integration of new backend, create/delete groups add members
</commit_message>
<xml_diff>
--- a/src/test_groups.xlsx
+++ b/src/test_groups.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="88">
   <si>
     <t>Table 1</t>
   </si>
@@ -161,9 +161,6 @@
   </si>
   <si>
     <t>Wednesday</t>
-  </si>
-  <si>
-    <t>Book Study</t>
   </si>
   <si>
     <t>Griff</t>
@@ -179,21 +176,12 @@
     <t>test group 1</t>
   </si>
   <si>
-    <t>Test description</t>
-  </si>
-  <si>
     <t>11306 County Line Rd, Madison, AL 35756</t>
   </si>
   <si>
     <t>Thursday</t>
   </si>
   <si>
-    <t>test@gmail.com</t>
-  </si>
-  <si>
-    <t>Don't Exist User</t>
-  </si>
-  <si>
     <t>test group 6</t>
   </si>
   <si>
@@ -218,9 +206,6 @@
     <t>18-30, 31-55, 55+</t>
   </si>
   <si>
-    <t>Outdoor</t>
-  </si>
-  <si>
     <t>Alex</t>
   </si>
   <si>
@@ -233,12 +218,6 @@
     <t>11:30 AM</t>
   </si>
   <si>
-    <t>Prayer</t>
-  </si>
-  <si>
-    <t>Finance</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -257,18 +236,12 @@
     <t>6:00 PM</t>
   </si>
   <si>
-    <t>Sp</t>
-  </si>
-  <si>
     <t>Friday</t>
   </si>
   <si>
     <t>7:00 AM</t>
   </si>
   <si>
-    <t>Outreach</t>
-  </si>
-  <si>
     <t>18-30</t>
   </si>
   <si>
@@ -285,6 +258,27 @@
   </si>
   <si>
     <t>Online</t>
+  </si>
+  <si>
+    <t>Ben Davis</t>
+  </si>
+  <si>
+    <t>Test description 1</t>
+  </si>
+  <si>
+    <t>Test description 2</t>
+  </si>
+  <si>
+    <t>Test description 3</t>
+  </si>
+  <si>
+    <t>Test description 4</t>
+  </si>
+  <si>
+    <t>Test description 5</t>
+  </si>
+  <si>
+    <t>Test description 6</t>
   </si>
 </sst>
 </file>
@@ -520,7 +514,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -562,9 +556,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="7" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -885,42 +876,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:27">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
-      <c r="Y1" s="19"/>
-      <c r="Z1" s="19"/>
-      <c r="AA1" s="19"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="18"/>
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18"/>
+      <c r="AA1" s="18"/>
     </row>
     <row r="2" spans="1:27" ht="153">
       <c r="A2" s="4" t="s">
@@ -1010,11 +1001,13 @@
         <v>13507637</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>50</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="15" t="s">
-        <v>57</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="7" t="b">
@@ -1022,7 +1015,7 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>34</v>
@@ -1034,16 +1027,16 @@
         <v>42</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
       <c r="P3" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="R3" s="2" t="s">
         <v>36</v>
@@ -1052,20 +1045,20 @@
         <v>43</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="U3" s="1"/>
       <c r="V3" s="1" t="s">
         <v>30</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="Z3" s="1" t="s">
         <v>32</v>
@@ -1074,18 +1067,18 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="63.75">
+    <row r="4" spans="1:27" ht="242.25">
       <c r="A4" s="8">
         <v>13511836</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>50</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>51</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="10" t="b">
@@ -1093,7 +1086,7 @@
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>34</v>
@@ -1105,19 +1098,19 @@
         <v>32</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
       <c r="O4" s="10"/>
       <c r="P4" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>54</v>
+        <v>83</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="S4" s="2" t="s">
         <v>43</v>
@@ -1133,10 +1126,10 @@
         <v>39</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="Z4" s="2" t="s">
         <v>33</v>
@@ -1145,18 +1138,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="63.75">
+    <row r="5" spans="1:27" ht="242.25">
       <c r="A5" s="11">
         <v>13562419</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>70</v>
+        <v>64</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>65</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="14" t="b">
@@ -1164,7 +1157,7 @@
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>40</v>
@@ -1176,32 +1169,32 @@
         <v>42</v>
       </c>
       <c r="L5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="M5" s="15" t="s">
         <v>50</v>
-      </c>
-      <c r="M5" s="16" t="s">
-        <v>51</v>
       </c>
       <c r="N5" s="14"/>
       <c r="O5" s="3" t="s">
         <v>41</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="S5" s="3" t="s">
         <v>37</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V5" s="3" t="s">
         <v>30</v>
@@ -1210,28 +1203,30 @@
         <v>31</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y5" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z5" s="3" t="s">
-        <v>33</v>
+        <v>71</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="AA5" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="63.75">
+    <row r="6" spans="1:27" ht="242.25">
       <c r="A6" s="11">
         <v>13562476</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" s="3"/>
+        <v>63</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="D6" s="16" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="14" t="b">
@@ -1239,7 +1234,7 @@
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>40</v>
@@ -1248,10 +1243,10 @@
         <v>44</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="14"/>
@@ -1259,13 +1254,13 @@
         <v>44</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="S6" s="3" t="s">
         <v>29</v>
@@ -1281,10 +1276,10 @@
         <v>45</v>
       </c>
       <c r="X6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y6" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="Y6" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="Z6" s="3" t="s">
         <v>33</v>
@@ -1293,18 +1288,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="63.75">
+    <row r="7" spans="1:27" ht="242.25">
       <c r="A7" s="11">
         <v>13562907</v>
       </c>
       <c r="B7" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>50</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>51</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="14" t="b">
@@ -1312,7 +1307,7 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>46</v>
@@ -1324,19 +1319,19 @@
         <v>32</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="M7" s="14"/>
       <c r="N7" s="14"/>
       <c r="O7" s="14"/>
       <c r="P7" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>54</v>
+        <v>86</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="S7" s="3" t="s">
         <v>37</v>
@@ -1354,10 +1349,10 @@
         <v>48</v>
       </c>
       <c r="X7" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y7" s="3" t="s">
-        <v>49</v>
+        <v>71</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="Z7" s="3" t="s">
         <v>32</v>
@@ -1366,18 +1361,18 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="63.75">
+    <row r="8" spans="1:27" ht="242.25">
       <c r="A8" s="11">
         <v>13563028</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="14" t="b">
@@ -1385,7 +1380,7 @@
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>46</v>
@@ -1397,38 +1392,38 @@
         <v>42</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="M8" s="14"/>
       <c r="N8" s="14"/>
       <c r="O8" s="14"/>
       <c r="P8" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="S8" s="3" t="s">
         <v>29</v>
       </c>
       <c r="T8" s="3"/>
       <c r="U8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="V8" s="3" t="s">
         <v>30</v>
       </c>
       <c r="W8" s="3" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="X8" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y8" s="3" t="s">
-        <v>83</v>
+        <v>74</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="Z8" s="3" t="s">
         <v>33</v>
@@ -1445,13 +1440,13 @@
     <mergeCell ref="A1:AA1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="D4" r:id="rId2"/>
-    <hyperlink ref="D5" r:id="rId3"/>
-    <hyperlink ref="D6" r:id="rId4"/>
-    <hyperlink ref="D7" r:id="rId5"/>
-    <hyperlink ref="D8" r:id="rId6" display="kassievest@daystarchurch.tv"/>
-    <hyperlink ref="M5" r:id="rId7"/>
+    <hyperlink ref="D4" r:id="rId1"/>
+    <hyperlink ref="D5" r:id="rId2"/>
+    <hyperlink ref="D7" r:id="rId3"/>
+    <hyperlink ref="D8" r:id="rId4" display="kassievest@daystarchurch.tv"/>
+    <hyperlink ref="M5" r:id="rId5"/>
+    <hyperlink ref="D6" r:id="rId6"/>
+    <hyperlink ref="D3" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
complete integration for all settings except location
</commit_message>
<xml_diff>
--- a/src/test_groups.xlsx
+++ b/src/test_groups.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="86">
   <si>
     <t>Table 1</t>
   </si>
@@ -103,9 +103,6 @@
     <t>S</t>
   </si>
   <si>
-    <t>Women</t>
-  </si>
-  <si>
     <t>Weekly</t>
   </si>
   <si>
@@ -127,9 +124,6 @@
     <t>All ages welcome</t>
   </si>
   <si>
-    <t>Co-ed (Both Men and Women welcome)</t>
-  </si>
-  <si>
     <t>In Home</t>
   </si>
   <si>
@@ -143,9 +137,6 @@
   </si>
   <si>
     <t>yes</t>
-  </si>
-  <si>
-    <t>Men</t>
   </si>
   <si>
     <t>2XL</t>
@@ -254,9 +245,6 @@
     <t>Griff Perry</t>
   </si>
   <si>
-    <t>Bible Study, Prayer, Freedom, Marriage, Finance, Outreach, Fitness/Health, Families, Fun/Hangout/Fellowship, Students, College Students, Other, Outdoor, Kids</t>
-  </si>
-  <si>
     <t>Online</t>
   </si>
   <si>
@@ -279,6 +267,12 @@
   </si>
   <si>
     <t>Test description 6</t>
+  </si>
+  <si>
+    <t>Bible Study, Prayer, Freedom, Marriage, Finance, Outreach, Fitness/Health, Families, Fun/Hangout/Fellowship, College Students, Outdoor, Kids</t>
+  </si>
+  <si>
+    <t>Co-ed</t>
   </si>
 </sst>
 </file>
@@ -876,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="H8" workbookViewId="0">
+      <selection activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -996,18 +990,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="242.25">
+    <row r="3" spans="1:27" ht="216.75">
       <c r="A3" s="5">
         <v>13507637</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="7" t="b">
@@ -1015,70 +1009,70 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>28</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
       <c r="P3" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="U3" s="1"/>
       <c r="V3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="Z3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AA3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AA3" s="1" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="4" spans="1:27" ht="242.25">
+    <row r="4" spans="1:27" ht="216.75">
       <c r="A4" s="8">
         <v>13511836</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="10" t="b">
@@ -1086,70 +1080,70 @@
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="K4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
       <c r="O4" s="10"/>
       <c r="P4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="R4" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="Q4" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>43</v>
+      <c r="S4" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="U4" s="10"/>
       <c r="V4" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AA4" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="242.25">
+    <row r="5" spans="1:27" ht="216.75">
       <c r="A5" s="11">
         <v>13562419</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="14" t="b">
@@ -1157,76 +1151,76 @@
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="L5" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="M5" s="15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="N5" s="14"/>
       <c r="O5" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="Q5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y5" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="R5" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="S5" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="U5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="V5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="W5" s="3" t="s">
+      <c r="Z5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="X5" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="Y5" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="Z5" s="1" t="s">
-        <v>32</v>
-      </c>
       <c r="AA5" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="242.25">
+    <row r="6" spans="1:27" ht="216.75">
       <c r="A6" s="11">
         <v>13562476</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="14" t="b">
@@ -1234,72 +1228,72 @@
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="14"/>
       <c r="O6" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="Q6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="S6" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="R6" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="T6" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="U6" s="3"/>
       <c r="V6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="W6" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="X6" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="Z6" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AA6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="242.25">
+    <row r="7" spans="1:27" ht="216.75">
       <c r="A7" s="11">
         <v>13562907</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="14" t="b">
@@ -1307,72 +1301,72 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="M7" s="14"/>
       <c r="N7" s="14"/>
       <c r="O7" s="14"/>
       <c r="P7" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>37</v>
+        <v>85</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="V7" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="X7" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="Z7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="AA7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="242.25">
+    <row r="8" spans="1:27" ht="216.75">
       <c r="A8" s="11">
         <v>13563028</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="14" t="b">
@@ -1380,56 +1374,56 @@
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="M8" s="14"/>
       <c r="N8" s="14"/>
       <c r="O8" s="14"/>
       <c r="P8" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>29</v>
+        <v>85</v>
       </c>
       <c r="T8" s="3"/>
       <c r="U8" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="V8" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="W8" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="X8" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="Z8" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AA8" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:27">

</xml_diff>

<commit_message>
Fix vague tags names
</commit_message>
<xml_diff>
--- a/src/test_groups.xlsx
+++ b/src/test_groups.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="88">
   <si>
     <t>Table 1</t>
   </si>
@@ -103,6 +103,9 @@
     <t>S</t>
   </si>
   <si>
+    <t>Women</t>
+  </si>
+  <si>
     <t>Weekly</t>
   </si>
   <si>
@@ -137,6 +140,9 @@
   </si>
   <si>
     <t>yes</t>
+  </si>
+  <si>
+    <t>Men</t>
   </si>
   <si>
     <t>2XL</t>
@@ -269,10 +275,10 @@
     <t>Test description 6</t>
   </si>
   <si>
-    <t>Bible Study, Prayer, Freedom, Marriage, Finance, Outreach, Fitness/Health, Families, Fun/Hangout/Fellowship, College Students, Outdoor, Kids</t>
-  </si>
-  <si>
     <t>Co-ed</t>
+  </si>
+  <si>
+    <t>Bible Study, Prayer, Freedom, Marriage, Finance, Outreach, Fitness/Health, Families, Fun/Hangout/Fellowship, Students, Other, College Students, Outdoor, Kids</t>
   </si>
 </sst>
 </file>
@@ -990,18 +996,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="216.75">
+    <row r="3" spans="1:27" ht="242.25">
       <c r="A3" s="5">
         <v>13507637</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="7" t="b">
@@ -1009,70 +1015,70 @@
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>28</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="M3" s="7"/>
       <c r="N3" s="7"/>
       <c r="O3" s="7"/>
       <c r="P3" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="Q3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="T3" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="U3" s="1"/>
       <c r="V3" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="W3" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="X3" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="Z3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="216.75">
+    <row r="4" spans="1:27" ht="242.25">
       <c r="A4" s="8">
         <v>13511836</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="10" t="b">
@@ -1080,70 +1086,70 @@
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
       <c r="O4" s="10"/>
       <c r="P4" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="U4" s="10"/>
       <c r="V4" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="Z4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AA4" s="2" t="s">
-        <v>31</v>
-      </c>
     </row>
-    <row r="5" spans="1:27" ht="216.75">
+    <row r="5" spans="1:27" ht="242.25">
       <c r="A5" s="11">
         <v>13562419</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="14" t="b">
@@ -1151,76 +1157,76 @@
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="M5" s="15" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="N5" s="14"/>
       <c r="O5" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="R5" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>85</v>
+        <v>42</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="V5" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="W5" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="Z5" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AA5" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="216.75">
+    <row r="6" spans="1:27" ht="242.25">
       <c r="A6" s="11">
         <v>13562476</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="14" t="b">
@@ -1228,72 +1234,72 @@
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="14"/>
       <c r="O6" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="U6" s="3"/>
       <c r="V6" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="W6" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="X6" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="Z6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AA6" s="3" t="s">
-        <v>31</v>
-      </c>
     </row>
-    <row r="7" spans="1:27" ht="216.75">
+    <row r="7" spans="1:27" ht="242.25">
       <c r="A7" s="11">
         <v>13562907</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="14" t="b">
@@ -1301,72 +1307,72 @@
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="J7" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="K7" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="M7" s="14"/>
       <c r="N7" s="14"/>
       <c r="O7" s="14"/>
       <c r="P7" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="T7" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="U7" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="V7" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="X7" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="Z7" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AA7" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="216.75">
+    <row r="8" spans="1:27" ht="242.25">
       <c r="A8" s="11">
         <v>13563028</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="14" t="b">
@@ -1374,56 +1380,56 @@
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="M8" s="14"/>
       <c r="N8" s="14"/>
       <c r="O8" s="14"/>
       <c r="P8" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>85</v>
+        <v>29</v>
       </c>
       <c r="T8" s="3"/>
       <c r="U8" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="V8" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="W8" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="X8" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="Z8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA8" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="AA8" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:27">

</xml_diff>

<commit_message>
Add group location if api key supports
</commit_message>
<xml_diff>
--- a/src/test_groups.xlsx
+++ b/src/test_groups.xlsx
@@ -876,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AA12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H8" workbookViewId="0">
-      <selection activeCell="Y8" sqref="Y8"/>
+    <sheetView tabSelected="1" topLeftCell="H3" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1045,7 +1045,7 @@
         <v>42</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>78</v>
+        <v>37</v>
       </c>
       <c r="U3" s="1"/>
       <c r="V3" s="1" t="s">

</xml_diff>